<commit_message>
Updating results file and moving model to folder
</commit_message>
<xml_diff>
--- a/Roll.xlsx
+++ b/Roll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\ziknet-trends-rolling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31EAD8F-5AFF-4E29-A8C6-406941D034E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050E5073-A8DD-486E-8D59-0BD467438AE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{DE36917B-B94A-4BEB-8135-296988929F04}"/>
   </bookViews>
@@ -139,18 +139,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -471,7 +465,7 @@
   <dimension ref="A10:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:D23"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -513,28 +507,28 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1">
-        <v>30.56</v>
-      </c>
-      <c r="D12" s="1">
-        <v>13.73</v>
-      </c>
-      <c r="E12" s="1">
-        <v>12.18</v>
-      </c>
-      <c r="F12" s="1">
-        <v>60.74</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="C12" s="3">
+        <v>9.15</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7.09</v>
+      </c>
+      <c r="E12" s="3">
+        <v>13.23</v>
+      </c>
+      <c r="F12" s="3">
+        <v>29.24</v>
+      </c>
+      <c r="H12" s="2">
         <v>42.09</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>63.75</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>76.989999999999995</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <v>87.19</v>
       </c>
     </row>
@@ -542,28 +536,28 @@
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13">
-        <v>13.84</v>
-      </c>
-      <c r="D13">
-        <v>18.45</v>
-      </c>
-      <c r="E13">
-        <v>3.78</v>
-      </c>
-      <c r="F13">
-        <v>0.84</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="C13" s="3">
+        <v>1.65</v>
+      </c>
+      <c r="D13" s="3">
+        <v>3.14</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="F13" s="3">
+        <v>7.47</v>
+      </c>
+      <c r="H13" s="2">
         <v>7.58</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>8.92</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>7.13</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <v>9.16</v>
       </c>
     </row>
@@ -571,28 +565,28 @@
       <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="C14">
-        <v>171.51</v>
-      </c>
-      <c r="D14">
-        <v>141.63999999999999</v>
-      </c>
-      <c r="E14">
-        <v>87.25</v>
-      </c>
-      <c r="F14">
-        <v>140.71</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="C14" s="3">
+        <v>686.17</v>
+      </c>
+      <c r="D14" s="3">
+        <v>484.28</v>
+      </c>
+      <c r="E14" s="3">
+        <v>833.86</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2251.3000000000002</v>
+      </c>
+      <c r="H14" s="2">
         <v>353.59</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>377.57</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <v>412.69</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <v>429.44</v>
       </c>
     </row>
@@ -600,28 +594,28 @@
       <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C15">
-        <v>185.45</v>
-      </c>
-      <c r="D15">
-        <v>145.1</v>
-      </c>
-      <c r="E15">
-        <v>113.48</v>
-      </c>
-      <c r="F15">
-        <v>110.77</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="C15" s="3">
+        <v>190.98</v>
+      </c>
+      <c r="D15" s="3">
+        <v>242.99</v>
+      </c>
+      <c r="E15" s="3">
+        <v>336.6</v>
+      </c>
+      <c r="F15" s="3">
+        <v>477.42</v>
+      </c>
+      <c r="H15" s="2">
         <v>211.58</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <v>217.15</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <v>218.68</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="1">
         <v>214.42</v>
       </c>
     </row>
@@ -629,28 +623,28 @@
       <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="C16">
-        <v>39.729999999999997</v>
-      </c>
-      <c r="D16">
-        <v>95.97</v>
-      </c>
-      <c r="E16">
-        <v>5.12</v>
-      </c>
-      <c r="F16">
-        <v>76.92</v>
-      </c>
-      <c r="H16" s="3">
+      <c r="C16" s="3">
+        <v>12.98</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.83</v>
+      </c>
+      <c r="E16" s="3">
+        <v>17.27</v>
+      </c>
+      <c r="F16" s="3">
+        <v>16.32</v>
+      </c>
+      <c r="H16" s="2">
         <v>278.43</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <v>291.10000000000002</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
         <v>316.01</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="1">
         <v>313.43</v>
       </c>
     </row>
@@ -663,28 +657,28 @@
       <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="5">
-        <v>674.46</v>
-      </c>
-      <c r="D19" s="5">
-        <v>2272.0100000000002</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1945.85</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2082.92</v>
-      </c>
-      <c r="H19" s="2">
+      <c r="C19" s="3">
+        <v>545.24</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2345.58</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3075.61</v>
+      </c>
+      <c r="F19" s="3">
+        <v>4818.71</v>
+      </c>
+      <c r="H19" s="1">
         <v>643.80999999999995</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="1">
         <v>1969.53</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
         <v>3901.63</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="1">
         <v>7119.83</v>
       </c>
     </row>
@@ -692,28 +686,28 @@
       <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="5">
-        <v>469.77</v>
-      </c>
-      <c r="D20" s="5">
-        <v>1325.92</v>
-      </c>
-      <c r="E20" s="4">
-        <v>5546.5</v>
-      </c>
-      <c r="F20" s="1">
-        <v>7220.92</v>
-      </c>
-      <c r="H20" s="2">
+      <c r="C20" s="3">
+        <v>267.33</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1450.17</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2930.08</v>
+      </c>
+      <c r="F20" s="3">
+        <v>3998.39</v>
+      </c>
+      <c r="H20" s="1">
         <v>563.09</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <v>2676.19</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="1">
         <v>6841.56</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1">
         <v>9646.2099999999991</v>
       </c>
     </row>
@@ -721,28 +715,28 @@
       <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="5">
-        <v>75.930000000000007</v>
-      </c>
-      <c r="D21" s="5">
-        <v>317.89999999999998</v>
-      </c>
-      <c r="E21" s="4">
-        <v>872.98</v>
-      </c>
-      <c r="F21" s="4">
-        <v>474.77</v>
-      </c>
-      <c r="H21" s="2">
+      <c r="C21" s="3">
+        <v>88.12</v>
+      </c>
+      <c r="D21" s="3">
+        <v>758.22</v>
+      </c>
+      <c r="E21" s="3">
+        <v>473.21</v>
+      </c>
+      <c r="F21" s="3">
+        <v>624.59</v>
+      </c>
+      <c r="H21" s="1">
         <v>131.58000000000001</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="1">
         <v>397.9</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="1">
         <v>847.8</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="1">
         <v>909.82</v>
       </c>
     </row>
@@ -750,28 +744,28 @@
       <c r="B22" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="5">
-        <v>2388.9499999999998</v>
-      </c>
-      <c r="D22" s="5">
-        <v>7009.92</v>
-      </c>
-      <c r="E22" s="4">
-        <v>7601.3</v>
-      </c>
-      <c r="F22" s="4">
-        <v>7507.85</v>
-      </c>
-      <c r="H22" s="2">
+      <c r="C22" s="3">
+        <v>1557.66</v>
+      </c>
+      <c r="D22" s="3">
+        <v>6159.84</v>
+      </c>
+      <c r="E22" s="3">
+        <v>6899.08</v>
+      </c>
+      <c r="F22" s="3">
+        <v>6953.07</v>
+      </c>
+      <c r="H22" s="1">
         <v>1214.3900000000001</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="1">
         <v>6604.44</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="1">
         <v>10591.64</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1">
         <v>13530.96</v>
       </c>
     </row>
@@ -779,28 +773,28 @@
       <c r="B23" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="5">
-        <v>43.08</v>
-      </c>
-      <c r="D23" s="5">
-        <v>130.16999999999999</v>
-      </c>
-      <c r="E23" s="4">
-        <v>225.7</v>
-      </c>
-      <c r="F23" s="4">
-        <v>220.45</v>
-      </c>
-      <c r="H23" s="2">
+      <c r="C23" s="3">
+        <v>30.59</v>
+      </c>
+      <c r="D23" s="3">
+        <v>145.41</v>
+      </c>
+      <c r="E23" s="3">
+        <v>138.63999999999999</v>
+      </c>
+      <c r="F23" s="3">
+        <v>299.86</v>
+      </c>
+      <c r="H23" s="1">
         <v>51.22</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="1">
         <v>140.38</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="1">
         <v>316.68</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="1">
         <v>337.81</v>
       </c>
     </row>

</xml_diff>